<commit_message>
field growth and weather readme
</commit_message>
<xml_diff>
--- a/Field growth and weather data/CGR3 field growth traits.xlsx
+++ b/Field growth and weather data/CGR3 field growth traits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGB\Documents\CGR3 manuscript\Data files for github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IGB\Documents\GitHub\CGR3-tobacco-2024\Field growth and weather data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>Genotype</t>
   </si>
@@ -35,9 +35,6 @@
     <t xml:space="preserve">Plant Number </t>
   </si>
   <si>
-    <t xml:space="preserve">Height </t>
-  </si>
-  <si>
     <t xml:space="preserve">Leaf # </t>
   </si>
   <si>
@@ -45,15 +42,6 @@
   </si>
   <si>
     <t>Leaf Area (m2)</t>
-  </si>
-  <si>
-    <t>Leaf Wt (g)</t>
-  </si>
-  <si>
-    <t>Stem Wt (g)</t>
-  </si>
-  <si>
-    <t>Root Wt (g)</t>
   </si>
   <si>
     <t>Above ground biomass (g)</t>
@@ -66,6 +54,21 @@
   </si>
   <si>
     <t>**Values to the right are averages by plot</t>
+  </si>
+  <si>
+    <t>Height (cm)</t>
+  </si>
+  <si>
+    <t>Height  (cm)</t>
+  </si>
+  <si>
+    <t>Leaf Weight (g)</t>
+  </si>
+  <si>
+    <t>Stem Weight (g)</t>
+  </si>
+  <si>
+    <t>Root Weight (g)</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
   <dimension ref="A1:Z121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,34 +427,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>0</v>
@@ -460,31 +463,31 @@
         <v>1</v>
       </c>
       <c r="P1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="Y1" s="5"/>
       <c r="Z1" s="5"/>
@@ -4937,7 +4940,7 @@
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -4976,7 +4979,7 @@
         <v>41.400000000000006</v>
       </c>
       <c r="N92" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O92">
         <v>1</v>
@@ -5020,7 +5023,7 @@
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -5059,7 +5062,7 @@
         <v>73.900000000000006</v>
       </c>
       <c r="N93" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O93">
         <v>2</v>
@@ -5103,7 +5106,7 @@
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -5142,7 +5145,7 @@
         <v>66.899999999999991</v>
       </c>
       <c r="N94" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O94">
         <v>3</v>
@@ -5186,7 +5189,7 @@
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -5225,7 +5228,7 @@
         <v>98.5</v>
       </c>
       <c r="N95" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O95">
         <v>4</v>
@@ -5269,7 +5272,7 @@
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -5308,7 +5311,7 @@
         <v>114.60000000000001</v>
       </c>
       <c r="N96" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O96">
         <v>5</v>
@@ -5352,7 +5355,7 @@
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B97" s="2">
         <v>2</v>
@@ -5391,7 +5394,7 @@
         <v>82.5</v>
       </c>
       <c r="N97" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O97">
         <v>6</v>
@@ -5435,7 +5438,7 @@
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B98" s="2">
         <v>2</v>
@@ -5476,7 +5479,7 @@
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B99">
         <v>2</v>
@@ -5517,7 +5520,7 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B100">
         <v>2</v>
@@ -5558,7 +5561,7 @@
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B101">
         <v>2</v>
@@ -5599,7 +5602,7 @@
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B102">
         <v>3</v>
@@ -5640,7 +5643,7 @@
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B103">
         <v>3</v>
@@ -5681,7 +5684,7 @@
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B104">
         <v>3</v>
@@ -5722,7 +5725,7 @@
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B105">
         <v>3</v>
@@ -5763,7 +5766,7 @@
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B106">
         <v>3</v>
@@ -5804,7 +5807,7 @@
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B107">
         <v>4</v>
@@ -5845,7 +5848,7 @@
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B108">
         <v>4</v>
@@ -5886,7 +5889,7 @@
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B109">
         <v>4</v>
@@ -5927,7 +5930,7 @@
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B110">
         <v>4</v>
@@ -5968,7 +5971,7 @@
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B111">
         <v>4</v>
@@ -6009,7 +6012,7 @@
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B112">
         <v>5</v>
@@ -6050,7 +6053,7 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B113">
         <v>5</v>
@@ -6091,7 +6094,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B114">
         <v>5</v>
@@ -6132,7 +6135,7 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B115">
         <v>5</v>
@@ -6173,7 +6176,7 @@
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B116">
         <v>5</v>
@@ -6214,7 +6217,7 @@
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B117">
         <v>6</v>
@@ -6255,7 +6258,7 @@
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B118">
         <v>6</v>
@@ -6296,7 +6299,7 @@
     </row>
     <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B119">
         <v>6</v>
@@ -6337,7 +6340,7 @@
     </row>
     <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B120">
         <v>6</v>
@@ -6378,7 +6381,7 @@
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B121" s="2">
         <v>6</v>

</xml_diff>